<commit_message>
feat: Implement global table candidate detection (BAT-26)
- Create table_candidates.py module with field-agnostic heuristics
- Implement TableCandidateBlock dataclass
- Add score_row_as_table_candidate() for row scoring
- Add find_table_candidate_rows() for grid scanning
- Add cluster_table_blocks() for row clustering
- Add detect_table_candidate_blocks() as main entry point
- Create comprehensive unit tests (31 tests, 95% coverage)
- Add field-agnostic verification tests (English vs Japanese)
- Enhance test fixtures with table data
- Update extraction/__init__.py with table detection exports
- Update plan-and-implement-ticket.md with git pull step
- All 219 tests pass with 94% overall coverage

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tests/fixtures/valid_template.xlsx
+++ b/tests/fixtures/valid_template.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,124 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Widget A</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Widget B</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>40</v>
+      </c>
+      <c r="D6" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Widget C</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>15</v>
+      </c>
+      <c r="C7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D7" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Widget D</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>50</v>
+      </c>
+      <c r="D8" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Widget E</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>12</v>
+      </c>
+      <c r="C9" t="n">
+        <v>35</v>
+      </c>
+      <c r="D9" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Widget F</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>20</v>
+      </c>
+      <c r="C10" t="n">
+        <v>28</v>
+      </c>
+      <c r="D10" t="n">
+        <v>560</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>